<commit_message>
[MOSIP-16645] Prereg json format UI spec corrected.
</commit_message>
<xml_diff>
--- a/deployment/v3/mosip/kernel/masterdata/xlsx/ui_spec.xlsx
+++ b/deployment/v3/mosip/kernel/masterdata/xlsx/ui_spec.xlsx
@@ -91,7 +91,381 @@
     <t xml:space="preserve">schema</t>
   </si>
   <si>
-    <t xml:space="preserve">{   "identity": {     "identity": [       {         "id": "IDSchemaVersion",         "description": "ID Schema Version",         "type": "number",         "controlType": null,         "fieldType": "default",         "inputRequired": false,         "validators": [],         "required": true       },       {         "id": "fullName",         "description": "Enter Full Name",         "labelName": {           "eng": "Full Name",           "fra": "Nom complet"         },         "controlType": "textbox",         "inputRequired": true,         "fieldType": "default",         "type": "simpleType",         "validators": [           {             "type": "regex",             "validator": "^(?=.{0,50}$).*",             "arguments": []           }         ],         "required": true,         "transliteration": true       },       {         "id": "dateOfBirth",         "description": "Enter DOB",         "labelName": {           "eng": "Date Of Birth",           "fra": "Date de naissance"         },         "controlType": "ageDate",         "inputRequired": true,         "fieldType": "default",         "type": "string",         "validators": [],         "required": true       },       {         "id": "gender",         "description": "Enter Gender",         "labelName": {           "eng": "Gender",           "fra": "Le genre"         },         "controlType": "dropdown",         "inputRequired": true,         "fieldType": "dynamic",         "type": "simpleType",         "validators": [],         "required": true       },       {         "id": "residenceStatus",         "description": "Residence status",         "labelName": {           "eng": "Residence Status",           "fra": "Statut de résidence"         },         "controlType": "dropdown",         "inputRequired": true,         "fieldType": "dynamic",         "type": "simpleType",         "validators": [],         "required": true       },       {         "id": "preferredLang",         "description": "Enter your preferred Language",         "labelName": {           "eng": "Preferred Language",           "fra": "langue préférée"         },         "controlType": "dropdown",         "inputRequired": true,         "fieldType": "dynamic",         "type": "string",         "validators": [],         "required": true       },       {         "id": "addressLine1",         "description": "addressLine1",         "labelName": {           "eng": "Address Line1",           "fra": "Address Line1"         },         "controlType": "textbox",         "inputRequired": true,         "fieldType": "default",         "type": "simpleType",         "validators": [           {             "type": "regex",             "validator": "^(?=.{0,50}$).*",             "arguments": []           }         ],         "required": true,         "transliteration": true       },       {         "id": "addressLine2",         "description": "addressLine2",         "labelName": {           "eng": "Address Line2",           "fra": "Adresse 2"         },         "controlType": "textbox",         "inputRequired": true,         "fieldType": "default",         "type": "simpleType",         "validators": [           {             "type": "regex",             "validator": "^(?=.{0,50}$).*",             "arguments": []           }         ],         "required": false,         "transliteration": true       },       {         "id": "addressLine3",         "description": "addressLine3",         "labelName": {           "eng": "Address Line3",           "fra": "Adresse 3"         ,         "controlType": "textbox",         "inputRequired": true,         "fieldType": "default",         "type": "simpleType",         "validators": [           {             "type": "regex",             "validator": "^(?=.{0,50}$).*",             "arguments": []           }         ],         "required": false,         "transliteration": true       },       {         "id": "region",         "description": "region",         "labelName": {           "eng": "Region",           "fra": "Région"         },         "controlType": "dropdown",         "inputRequired": true,         "fieldType": "default",         "type": "simpleType",         "validators": [           {             "type": "regex",             "validator": "^(?=.{0,50}$).*",             "arguments": []           }         ],         "required": true       },       {         "id": "province",         "description": "province",         "labelName": {           "eng": "Province",           "fra": "Province"         },         "controlType": "dropdown",         "inputRequired": true,         "fieldType": "default",         "type": "simpleType",         "validators": [           {             "type": "regex",             "validator": "^(?=.{0,50}$).*",             "arguments": []           }         ],         "required": true       },       {         "id": "city",         "description": "city",         "labelName": {           "eng": "City",           "fra": "Ville"         },         "controlType": "dropdown",         "inputRequired": true,         "fieldType": "default",         "type": "simpleType",         "validators": [           {             "type": "regex",             "validator": "^(?=.{0,50}$).*",             "arguments": []           }         ],         "required": true       },       {         "id": "zone",         "description": "zone",         "labelName": {           "eng": "Zone",           "fra": "Zone"         },         "controlType": "dropdown",         "inputRequired": true,         "fieldType": "default",         "type": "simpleType",         "validators": [],         "required": true       },       {         "id": "postalCode",         "description": "postalCode",         "labelName": {           "eng": "Postal Code",           "fra": "code postal"         },         "controlType": "dropdown",         "inputRequired": true,         "fieldType": "default",         "type": "string",         "validators": [           {             "type": "regex",             "validator": "^[(?i)A-Z0-9]{5}$|^NA$",             "arguments": []           }         ],         "required": true       },       {         "id": "phone",         "description": "phone",         "labelName": {           "eng": "Phone",           "fra": "Téléphone"         },         "controlType": "textbox",         "inputRequired": true,         "fieldType": "default",         "type": "string",         "validators": [           {             "type": "regex",             "validator": "^([6-9]{1})([0-9]{9})$",             "arguments": []           }         ],         "required": true       },       {         "id": "email",         "description": "email",         "labelName": {           "eng": "Email",           "fra": "Email"         },         "controlType": "textbox",         "inputRequired": true,         "fieldType": "default",         "type": "string",         "validators": [           {             "type": "regex",             "validator": "^[\\w-\\+]+(\\.[\\w]+)*@[\\w-]+(\\.[\\w]+)*(\\.[a-zA-Z]{2,})$",             "arguments": []           }         ],         "required": true       },       {         "id": "proofOfAddress",         "description": "proofOfAddress",         "labelName": {           "eng": "Address Proof",           "fra": "Address Proof"         },         "controlType": "fileupload",         "inputRequired": true,         "validators": [],         "subType": "POA",         "required": false       },       {         "id": "proofOfIdentity",         "description": "proofOfIdentity",         "labelName": {           "eng": "Identity Proof",           "fra": "Identity Proof"         },         "controlType": "fileupload",         "inputRequired": true,         "validators": [],         "subType": "POI",         "required": true       },       {         "id": "proofOfRelationship",         "description": "proofOfRelationship",         "labelName": {           "eng": "Relationship Proof",           "fra": "Relationship Proof"         },         "controlType": "fileupload",         "inputRequired": true,         "validators": [],         "subType": "POR",         "required": true       },       {         "id": "proofOfDateOfBirth",         "description": "proofOfDateOfBirth",         "labelName": {           "eng": "DOB Proof",           "fra": "DOB Proof"         },         "controlType": "fileupload",         "inputRequired": true,         "validators": [],         "subType": "POB",         "required": true       },       {         "id": "proofOfException",         "description": "proofOfException",         "labelName": {           "eng": "Exception Proof",           "fra": "Exception Proof"         },         "controlType": "fileupload",         "inputRequired": true,         "validators": [],         "subType": "POE",         "required": true       },       {         "id": "proofOfException-1",         "description": "proofOfException",         "labelName": {           "eng": "Exception Proof 2",           "fra": "Exception Proof 2"         },         "controlType": "fileupload",         "inputRequired": true,         "validators": [],         "subType": "POE",         "required": true       }     ],     "locationHierarchy": [       "region",       "province",       "city",       "zone",       "postalCode"     ]   } }</t>
+    <t xml:space="preserve">{
+  "identity": {
+    "identity": [
+      {
+        "id": "IDSchemaVersion",
+        "description": "ID Schema Version",
+        "type": "number",
+        "controlType": null,
+        "fieldType": "default",
+        "inputRequired": false,
+        "validators": [],
+        "required": true
+      },
+      {
+        "id": "fullName",
+        "description": "Enter Full Name",
+        "labelName": {
+          "eng": "Full Name",
+          "fra": "Nom complet"
+        },
+        "controlType": "textbox",
+        "inputRequired": true,
+        "fieldType": "default",
+        "type": "simpleType",
+        "validators": [
+          {
+            "type": "regex",
+            "validator": "^(?=.{0,50}$).*",
+            "arguments": []
+          }
+        ],
+        "required": true,
+        "transliteration": true
+      },
+      {
+        "id": "dateOfBirth",
+        "description": "Enter DOB",
+        "labelName": {
+          "eng": "Date Of Birth",
+          "fra": "Date de naissance"
+        },
+        "controlType": "ageDate",
+        "inputRequired": true,
+        "fieldType": "default",
+        "type": "string",
+        "validators": [],
+        "required": true
+      },
+      {
+        "id": "gender",
+        "description": "Enter Gender",
+        "labelName": {
+          "eng": "Gender",
+          "fra": "Le genre"
+        },
+        "controlType": "dropdown",
+        "inputRequired": true,
+        "fieldType": "dynamic",
+        "type": "simpleType",
+        "validators": [],
+        "required": true
+      },
+      {
+        "id": "residenceStatus",
+        "description": "Residence status",
+        "labelName": {
+          "eng": "Residence Status",
+          "fra": "Statut de résidence"
+        },
+        "controlType": "dropdown",
+        "inputRequired": true,
+        "fieldType": "dynamic",
+        "type": "simpleType",
+        "validators": [],
+        "required": true
+      },
+      {
+        "id": "preferredLang",
+        "description": "Enter your preferred Language",
+        "labelName": {
+          "eng": "Preferred Language",
+          "fra": "langue préférée"
+        },
+        "controlType": "dropdown",
+        "inputRequired": true,
+        "fieldType": "dynamic",
+        "type": "string",
+        "validators": [],
+        "required": true
+      },
+      {
+        "id": "addressLine1",
+        "description": "addressLine1",
+        "labelName": {
+          "eng": "Address Line1",
+          "fra": "Adresse 1"
+        },
+        "controlType": "textbox",
+        "inputRequired": true,
+        "fieldType": "default",
+        "type": "simpleType",
+        "validators": [
+          {
+            "type": "regex",
+            "validator": "^(?=.{0,50}$).*",
+            "arguments": []
+          }
+        ],
+        "required": true,
+        "transliteration": true
+      },
+      {
+        "id": "addressLine2",
+        "description": "addressLine2",
+        "labelName": {
+          "eng": "Address Line2",
+          "fra": "Adresse 2"
+        },
+        "controlType": "textbox",
+        "inputRequired": true,
+        "fieldType": "default",
+        "type": "simpleType",
+        "validators": [
+          {
+            "type": "regex",
+            "validator": "^(?=.{0,50}$).*",
+            "arguments": []
+          }
+        ],
+        "required": false,
+        "transliteration": true
+      },
+      {
+        "id": "addressLine3",
+        "description": "addressLine3",
+        "labelName": {
+          "eng": "Address Line3",
+          "fra": "Adresse 3"
+        },
+        "controlType": "textbox",
+        "inputRequired": true,
+        "fieldType": "default",
+        "type": "simpleType",
+        "validators": [
+          {
+            "type": "regex",
+            "validator": "^(?=.{0,50}$).*",
+            "arguments": []
+          }
+        ],
+        "required": false,
+        "transliteration": true
+      },
+      {
+        "id": "region",
+        "description": "region",
+        "labelName": {
+          "eng": "Region",
+          "fra": "Région"
+        },
+        "controlType": "dropdown",
+        "inputRequired": true,
+        "fieldType": "default",
+        "type": "simpleType",
+        "validators": [
+          {
+            "type": "regex",
+            "validator": "^(?=.{0,50}$).*",
+            "arguments": []
+          }
+        ],
+        "required": true
+      },
+      {
+        "id": "province",
+        "description": "province",
+        "labelName": {
+          "eng": "Province",
+          "fra": "Province"
+        },
+        "controlType": "dropdown",
+        "inputRequired": true,
+        "fieldType": "default",
+        "type": "simpleType",
+        "validators": [
+          {
+            "type": "regex",
+            "validator": "^(?=.{0,50}$).*",
+            "arguments": []
+          }
+        ],
+        "required": true
+      },
+      {
+        "id": "city",
+        "description": "city",
+        "labelName": {
+          "eng": "City",
+          "fra": "Ville"
+        },
+        "controlType": "dropdown",
+        "inputRequired": true,
+        "fieldType": "default",
+        "type": "simpleType",
+        "validators": [
+          {
+            "type": "regex",
+            "validator": "^(?=.{0,50}$).*",
+            "arguments": []
+          }
+        ],
+        "required": true
+      },
+      {
+        "id": "zone",
+        "description": "zone",
+        "labelName": {
+          "eng": "Zone",
+          "fra": "Zone"
+        },
+        "controlType": "dropdown",
+        "inputRequired": true,
+        "fieldType": "default",
+        "type": "simpleType",
+        "validators": [],
+        "required": true
+      },
+      {
+        "id": "postalCode",
+        "description": "postalCode",
+        "labelName": {
+          "eng": "Postal Code",
+          "fra": "code postal"
+        },
+        "controlType": "dropdown",
+        "inputRequired": true,
+        "fieldType": "default",
+        "type": "string",
+        "validators": [
+          {
+            "type": "regex",
+            "validator": "^[(?i)A-Z0-9]{5}$|^NA$",
+            "arguments": []
+          }
+        ],
+        "required": true
+      },
+      {
+        "id": "phone",
+        "description": "phone",
+        "labelName": {
+          "eng": "Phone",
+          "fra": "Téléphone"
+        },
+        "controlType": "textbox",
+        "inputRequired": true,
+        "fieldType": "default",
+        "type": "string",
+        "validators": [
+          {
+            "type": "regex",
+            "validator": "^([6-9]{1})([0-9]{9})$",
+            "arguments": []
+          }
+        ],
+        "required": true
+      },
+      {
+        "id": "email",
+        "description": "email",
+        "labelName": {
+          "eng": "Email",
+          "fra": "Email"
+        },
+        "controlType": "textbox",
+        "inputRequired": true,
+        "fieldType": "default",
+        "type": "string",
+        "validators": [
+          {
+            "type": "regex",
+            "validator": "^[\\w-\\+]+(\\.[\\w]+)*@[\\w-]+(\\.[\\w]+)*(\\.[a-zA-Z]{2,})$",
+            "arguments": []
+          }
+        ],
+        "required": true
+      },
+      {
+        "id": "proofOfAddress",
+        "description": "proofOfAddress",
+        "labelName": {
+          "fra": "Address Proof",
+          "eng": "Address Proof"
+        },
+        "controlType": "fileupload",
+        "inputRequired": true,
+        "validators": [],
+        "subType": "POA",
+        "required": false
+      },
+      {
+        "id": "proofOfIdentity",
+        "description": "proofOfIdentity",
+        "labelName": {
+          "fra": "Identity Proof",
+          "eng": "Identity Proof"
+        },
+        "controlType": "fileupload",
+        "inputRequired": true,
+        "validators": [],
+        "subType": "POI",
+        "required": true
+      },
+      {
+        "id": "proofOfRelationship",
+        "description": "proofOfRelationship",
+        "labelName": {
+          "fra": "Relationship Proof",
+          "eng": "Relationship Proof"
+        },
+        "controlType": "fileupload",
+        "inputRequired": true,
+        "validators": [],
+        "subType": "POR",
+        "required": true
+      },
+      {
+        "id": "proofOfDateOfBirth",
+        "description": "proofOfDateOfBirth",
+        "labelName": {
+          "fra": "DOB Proof",
+          "eng": "DOB Proof"
+        },
+        "controlType": "fileupload",
+        "inputRequired": true,
+        "validators": [],
+        "subType": "POB",
+        "required": true
+      },
+      {
+        "id": "proofOfException",
+        "description": "proofOfException",
+        "labelName": {
+          "fra": "Exception Proof",
+          "eng": "Exception Proof"
+        },
+        "controlType": "fileupload",
+        "inputRequired": true,
+        "validators": [],
+        "subType": "POE",
+        "required": true
+      },
+      {
+        "id": "proofOfException-1",
+        "description": "proofOfException",
+        "labelName": {
+          "fra": "Exception Proof 2",
+          "eng": "Exception Proof 2"
+        },
+        "controlType": "fileupload",
+        "inputRequired": true,
+        "validators": [],
+        "subType": "POE",
+        "required": true
+      }
+    ],
+    "locationHierarchy": [
+      "region",
+      "province",
+      "city",
+      "zone",
+      "postalCode"
+    ]
+  }
+}</t>
   </si>
   <si>
     <t xml:space="preserve">now()</t>
@@ -305,10 +679,11 @@
       <charset val="1"/>
     </font>
     <font>
-      <sz val="11"/>
+      <sz val="10"/>
       <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
+      <name val="Menlo-Regular"/>
+      <family val="0"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="11"/>
@@ -367,7 +742,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -376,7 +751,11 @@
       <alignment horizontal="center" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -403,11 +782,11 @@
   </sheetPr>
   <dimension ref="A1:R5"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="H1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="P6" activeCellId="0" sqref="P6"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A2" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="G2" activeCellId="0" sqref="G2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.515625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.53515625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="24.1"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="15.4"/>
@@ -472,7 +851,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="29.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="3276.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
         <v>18</v>
       </c>
@@ -491,7 +870,7 @@
       <c r="F2" s="0" t="s">
         <v>22</v>
       </c>
-      <c r="G2" s="0" t="s">
+      <c r="G2" s="2" t="s">
         <v>23</v>
       </c>
       <c r="H2" s="0" t="n">
@@ -553,7 +932,7 @@
       <c r="I3" s="0" t="n">
         <v>0.1</v>
       </c>
-      <c r="J3" s="2" t="s">
+      <c r="J3" s="3" t="s">
         <v>24</v>
       </c>
       <c r="K3" s="0" t="s">
@@ -606,7 +985,7 @@
       <c r="I4" s="0" t="n">
         <v>0.1</v>
       </c>
-      <c r="J4" s="2" t="s">
+      <c r="J4" s="3" t="s">
         <v>24</v>
       </c>
       <c r="K4" s="0" t="s">
@@ -650,7 +1029,7 @@
       <c r="F5" s="0" t="s">
         <v>22</v>
       </c>
-      <c r="G5" s="3" t="s">
+      <c r="G5" s="4" t="s">
         <v>44</v>
       </c>
       <c r="H5" s="0" t="n">
@@ -659,7 +1038,7 @@
       <c r="I5" s="0" t="n">
         <v>0.1</v>
       </c>
-      <c r="J5" s="2" t="s">
+      <c r="J5" s="3" t="s">
         <v>24</v>
       </c>
       <c r="K5" s="0" t="s">

</xml_diff>

<commit_message>
[MOSIP-16645] Preferred languages removed from PreReg UI specs.
</commit_message>
<xml_diff>
--- a/deployment/v3/mosip/kernel/masterdata/xlsx/ui_spec.xlsx
+++ b/deployment/v3/mosip/kernel/masterdata/xlsx/ui_spec.xlsx
@@ -164,20 +164,6 @@
         "inputRequired": true,
         "fieldType": "dynamic",
         "type": "simpleType",
-        "validators": [],
-        "required": true
-      },
-      {
-        "id": "preferredLang",
-        "description": "Enter your preferred Language",
-        "labelName": {
-          "eng": "Preferred Language",
-          "fra": "langue préférée"
-        },
-        "controlType": "dropdown",
-        "inputRequired": true,
-        "fieldType": "dynamic",
-        "type": "string",
         "validators": [],
         "required": true
       },
@@ -683,7 +669,6 @@
       <color rgb="FF000000"/>
       <name val="Menlo-Regular"/>
       <family val="0"/>
-      <charset val="1"/>
     </font>
     <font>
       <sz val="11"/>
@@ -742,13 +727,17 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
@@ -783,10 +772,10 @@
   <dimension ref="A1:R5"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A2" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G2" activeCellId="0" sqref="G2"/>
+      <selection pane="topLeft" activeCell="D2" activeCellId="0" sqref="D2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.53515625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="24.1"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="15.4"/>
@@ -861,7 +850,7 @@
       <c r="C2" s="0" t="s">
         <v>19</v>
       </c>
-      <c r="D2" s="0" t="s">
+      <c r="D2" s="2" t="s">
         <v>20</v>
       </c>
       <c r="E2" s="0" t="s">
@@ -870,7 +859,7 @@
       <c r="F2" s="0" t="s">
         <v>22</v>
       </c>
-      <c r="G2" s="2" t="s">
+      <c r="G2" s="3" t="s">
         <v>23</v>
       </c>
       <c r="H2" s="0" t="n">
@@ -932,7 +921,7 @@
       <c r="I3" s="0" t="n">
         <v>0.1</v>
       </c>
-      <c r="J3" s="3" t="s">
+      <c r="J3" s="4" t="s">
         <v>24</v>
       </c>
       <c r="K3" s="0" t="s">
@@ -985,7 +974,7 @@
       <c r="I4" s="0" t="n">
         <v>0.1</v>
       </c>
-      <c r="J4" s="3" t="s">
+      <c r="J4" s="4" t="s">
         <v>24</v>
       </c>
       <c r="K4" s="0" t="s">
@@ -1020,7 +1009,7 @@
       <c r="C5" s="0" t="s">
         <v>30</v>
       </c>
-      <c r="D5" s="0" t="s">
+      <c r="D5" s="2" t="s">
         <v>42</v>
       </c>
       <c r="E5" s="0" t="s">
@@ -1029,7 +1018,7 @@
       <c r="F5" s="0" t="s">
         <v>22</v>
       </c>
-      <c r="G5" s="4" t="s">
+      <c r="G5" s="5" t="s">
         <v>44</v>
       </c>
       <c r="H5" s="0" t="n">
@@ -1038,7 +1027,7 @@
       <c r="I5" s="0" t="n">
         <v>0.1</v>
       </c>
-      <c r="J5" s="3" t="s">
+      <c r="J5" s="4" t="s">
         <v>24</v>
       </c>
       <c r="K5" s="0" t="s">

</xml_diff>